<commit_message>
Add results of K2, TAN and Hill Climbing
</commit_message>
<xml_diff>
--- a/evidence/k2-tan-results.xlsx
+++ b/evidence/k2-tan-results.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
   <si>
     <t xml:space="preserve">K2</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">TAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hill Climber</t>
   </si>
 </sst>
 </file>
@@ -60,6 +63,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -149,18 +153,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="topLeft" activeCell="G36" activeCellId="0" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.6683673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -469,6 +474,228 @@
       </c>
       <c r="E20" s="2" t="n">
         <v>0.1668</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>0.376883</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <f aca="false">1-C26</f>
+        <v>0.623117</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>0.2849</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>0.3306</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>0.761713</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="false">1-C27</f>
+        <v>0.238287</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>0.7102</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>0.188</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>0.760475</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="false">1-C28</f>
+        <v>0.239525</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>0.7082</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <v>0.1852</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>0.40516</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">1-C30</f>
+        <v>0.59484</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>0.3183</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>0.3322</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>0.79969</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">1-C31</f>
+        <v>0.20031</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0.7566</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>0.176</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>0.795253</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <f aca="false">1-C32</f>
+        <v>0.204747</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>0.7508</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>0.1736</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>0.409288</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <f aca="false">1-C34</f>
+        <v>0.590712</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>0.3231</v>
+      </c>
+      <c r="F34" s="0" t="n">
+        <v>0.3358</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>0.817023</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="false">1-C35</f>
+        <v>0.182977</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>0.7778</v>
+      </c>
+      <c r="F35" s="0" t="n">
+        <v>0.1719</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>0.801238</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">1-C36</f>
+        <v>0.198762</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>0.758</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>0.173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>